<commit_message>
GUI Formatting and Dimension Label
</commit_message>
<xml_diff>
--- a/Sunken Temple/Ideas/Guardian_Game_Item_Combos.xlsx
+++ b/Sunken Temple/Ideas/Guardian_Game_Item_Combos.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="10515" windowHeight="11565"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="21020" windowHeight="14060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -387,165 +392,165 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -553,18 +558,18 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -572,17 +577,17 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -592,7 +597,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -600,12 +605,12 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -614,50 +619,50 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -801,12 +806,54 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -821,48 +868,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1171,30 +1176,30 @@
       <selection activeCell="H9" sqref="H9:I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="4" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="20" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="20" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="3" customWidth="1"/>
-    <col min="10" max="10" width="2.7109375" customWidth="1"/>
+    <col min="10" max="10" width="2.6640625" customWidth="1"/>
     <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="9.1640625" customWidth="1"/>
     <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" customWidth="1"/>
+    <col min="18" max="18" width="9.1640625" customWidth="1"/>
     <col min="19" max="19" width="0" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="9.140625" customWidth="1"/>
+    <col min="22" max="22" width="9.1640625" customWidth="1"/>
     <col min="23" max="23" width="0" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="9.140625" customWidth="1"/>
+    <col min="26" max="26" width="9.1640625" customWidth="1"/>
     <col min="27" max="27" width="0" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="9.140625" customWidth="1"/>
+    <col min="30" max="30" width="9.1640625" customWidth="1"/>
     <col min="31" max="31" width="0" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="9.140625" customWidth="1"/>
+    <col min="34" max="34" width="9.1640625" customWidth="1"/>
     <col min="35" max="35" width="0" hidden="1" customWidth="1"/>
-    <col min="40" max="40" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" ht="15" hidden="1" customHeight="1">
       <c r="A1">
         <v>2</v>
       </c>
@@ -1217,12 +1222,12 @@
       <c r="P1" s="37"/>
       <c r="Q1" s="37"/>
     </row>
-    <row r="2" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" ht="15" thickBot="1">
       <c r="E2" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" ht="15" thickBot="1">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1233,49 +1238,49 @@
         <v>6</v>
       </c>
       <c r="K3" s="37"/>
-      <c r="L3" s="86" t="s">
+      <c r="L3" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="M3" s="87"/>
-      <c r="N3" s="88"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="92"/>
       <c r="O3" s="45"/>
-      <c r="P3" s="86" t="s">
+      <c r="P3" s="90" t="s">
         <v>71</v>
       </c>
-      <c r="Q3" s="87"/>
-      <c r="R3" s="88"/>
+      <c r="Q3" s="91"/>
+      <c r="R3" s="92"/>
       <c r="S3" s="45"/>
-      <c r="T3" s="86" t="s">
+      <c r="T3" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="U3" s="87"/>
-      <c r="V3" s="88"/>
+      <c r="U3" s="91"/>
+      <c r="V3" s="92"/>
       <c r="W3" s="45"/>
-      <c r="X3" s="86" t="s">
+      <c r="X3" s="90" t="s">
         <v>73</v>
       </c>
-      <c r="Y3" s="87"/>
-      <c r="Z3" s="88"/>
+      <c r="Y3" s="91"/>
+      <c r="Z3" s="92"/>
       <c r="AA3" s="45"/>
-      <c r="AB3" s="86" t="s">
+      <c r="AB3" s="90" t="s">
         <v>74</v>
       </c>
-      <c r="AC3" s="87"/>
-      <c r="AD3" s="88"/>
+      <c r="AC3" s="91"/>
+      <c r="AD3" s="92"/>
       <c r="AE3" s="45"/>
-      <c r="AF3" s="86" t="s">
+      <c r="AF3" s="90" t="s">
         <v>75</v>
       </c>
-      <c r="AG3" s="87"/>
-      <c r="AH3" s="88"/>
+      <c r="AG3" s="91"/>
+      <c r="AH3" s="92"/>
       <c r="AI3" s="45"/>
-      <c r="AJ3" s="86" t="s">
+      <c r="AJ3" s="90" t="s">
         <v>76</v>
       </c>
-      <c r="AK3" s="87"/>
-      <c r="AL3" s="88"/>
-    </row>
-    <row r="4" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AK3" s="91"/>
+      <c r="AL3" s="92"/>
+    </row>
+    <row r="4" spans="1:38" ht="15" thickBot="1">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1285,10 +1290,10 @@
       <c r="E4" s="20">
         <v>5</v>
       </c>
-      <c r="H4" s="89" t="s">
+      <c r="H4" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="I4" s="90"/>
+      <c r="I4" s="94"/>
       <c r="K4" t="s">
         <v>13</v>
       </c>
@@ -1332,7 +1337,7 @@
       <c r="AK4" s="56"/>
       <c r="AL4" s="58"/>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1345,10 +1350,10 @@
       <c r="G5" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="H5" s="96" t="s">
+      <c r="H5" s="80" t="s">
         <v>95</v>
       </c>
-      <c r="I5" s="97"/>
+      <c r="I5" s="81"/>
       <c r="K5" t="s">
         <v>32</v>
       </c>
@@ -1392,7 +1397,7 @@
       <c r="AK5" s="27"/>
       <c r="AL5" s="30"/>
     </row>
-    <row r="6" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" ht="15" thickBot="1">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1405,8 +1410,8 @@
       <c r="G6" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="H6" s="98"/>
-      <c r="I6" s="99"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="83"/>
       <c r="L6" s="22"/>
       <c r="M6" s="26"/>
       <c r="N6" s="35"/>
@@ -1447,7 +1452,7 @@
       <c r="AK6" s="24"/>
       <c r="AL6" s="31"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1460,10 +1465,10 @@
       <c r="G7" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="96" t="s">
+      <c r="H7" s="80" t="s">
         <v>94</v>
       </c>
-      <c r="I7" s="97"/>
+      <c r="I7" s="81"/>
       <c r="L7" s="22"/>
       <c r="M7" s="26"/>
       <c r="N7" s="35"/>
@@ -1504,7 +1509,7 @@
       <c r="AK7" s="28"/>
       <c r="AL7" s="32"/>
     </row>
-    <row r="8" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38" ht="15" thickBot="1">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1517,8 +1522,8 @@
       <c r="G8" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="H8" s="98"/>
-      <c r="I8" s="99"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="83"/>
       <c r="L8" s="22"/>
       <c r="M8" s="26"/>
       <c r="N8" s="35"/>
@@ -1559,7 +1564,7 @@
       <c r="AK8" s="25"/>
       <c r="AL8" s="33"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1572,10 +1577,10 @@
       <c r="G9" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="96" t="s">
+      <c r="H9" s="80" t="s">
         <v>92</v>
       </c>
-      <c r="I9" s="93"/>
+      <c r="I9" s="84"/>
       <c r="L9" s="22"/>
       <c r="M9" s="26"/>
       <c r="N9" s="35"/>
@@ -1616,7 +1621,7 @@
       <c r="AK9" s="29"/>
       <c r="AL9" s="34"/>
     </row>
-    <row r="10" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:38" ht="15" thickBot="1">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1629,8 +1634,8 @@
       <c r="G10" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="94"/>
-      <c r="I10" s="95"/>
+      <c r="H10" s="85"/>
+      <c r="I10" s="86"/>
       <c r="L10" s="22"/>
       <c r="M10" s="26"/>
       <c r="N10" s="35"/>
@@ -1665,7 +1670,7 @@
       <c r="AK10" s="26"/>
       <c r="AL10" s="35"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1678,10 +1683,10 @@
       <c r="G11" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="H11" s="92" t="s">
+      <c r="H11" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="I11" s="93"/>
+      <c r="I11" s="84"/>
       <c r="L11" s="22"/>
       <c r="M11" s="26"/>
       <c r="N11" s="35"/>
@@ -1716,7 +1721,7 @@
       <c r="AK11" s="26"/>
       <c r="AL11" s="35"/>
     </row>
-    <row r="12" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:38" ht="15" thickBot="1">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1729,8 +1734,8 @@
       <c r="G12" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="H12" s="94"/>
-      <c r="I12" s="95"/>
+      <c r="H12" s="85"/>
+      <c r="I12" s="86"/>
       <c r="L12" s="22"/>
       <c r="M12" s="26"/>
       <c r="N12" s="35"/>
@@ -1765,7 +1770,7 @@
       <c r="AK12" s="26"/>
       <c r="AL12" s="35"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1778,10 +1783,10 @@
       <c r="G13" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="H13" s="96" t="s">
+      <c r="H13" s="80" t="s">
         <v>93</v>
       </c>
-      <c r="I13" s="97"/>
+      <c r="I13" s="81"/>
       <c r="L13" s="22"/>
       <c r="M13" s="26"/>
       <c r="N13" s="35"/>
@@ -1816,7 +1821,7 @@
       <c r="AK13" s="26"/>
       <c r="AL13" s="35"/>
     </row>
-    <row r="14" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:38" ht="15" thickBot="1">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1829,8 +1834,8 @@
       <c r="G14" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="H14" s="98"/>
-      <c r="I14" s="99"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="83"/>
       <c r="L14" s="22"/>
       <c r="M14" s="26"/>
       <c r="N14" s="35"/>
@@ -1865,7 +1870,7 @@
       <c r="AK14" s="26"/>
       <c r="AL14" s="35"/>
     </row>
-    <row r="15" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:38" ht="15" thickBot="1">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1909,7 +1914,7 @@
       <c r="AK15" s="36"/>
       <c r="AL15" s="60"/>
     </row>
-    <row r="16" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:38" ht="15" thickBot="1">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1919,49 +1924,49 @@
       <c r="E16" s="20">
         <v>2</v>
       </c>
-      <c r="L16" s="81" t="s">
+      <c r="L16" s="95" t="s">
         <v>79</v>
       </c>
-      <c r="M16" s="82"/>
-      <c r="N16" s="83"/>
+      <c r="M16" s="96"/>
+      <c r="N16" s="97"/>
       <c r="O16" s="46"/>
-      <c r="P16" s="81" t="s">
+      <c r="P16" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="Q16" s="82"/>
-      <c r="R16" s="83"/>
+      <c r="Q16" s="96"/>
+      <c r="R16" s="97"/>
       <c r="S16" s="46"/>
-      <c r="T16" s="81" t="s">
+      <c r="T16" s="95" t="s">
         <v>77</v>
       </c>
-      <c r="U16" s="82"/>
-      <c r="V16" s="83"/>
+      <c r="U16" s="96"/>
+      <c r="V16" s="97"/>
       <c r="W16" s="46"/>
-      <c r="X16" s="81" t="s">
+      <c r="X16" s="95" t="s">
         <v>80</v>
       </c>
-      <c r="Y16" s="82"/>
-      <c r="Z16" s="83"/>
+      <c r="Y16" s="96"/>
+      <c r="Z16" s="97"/>
       <c r="AA16" s="46"/>
-      <c r="AB16" s="81" t="s">
+      <c r="AB16" s="95" t="s">
         <v>81</v>
       </c>
-      <c r="AC16" s="82"/>
-      <c r="AD16" s="83"/>
+      <c r="AC16" s="96"/>
+      <c r="AD16" s="97"/>
       <c r="AE16" s="46"/>
-      <c r="AF16" s="81" t="s">
+      <c r="AF16" s="95" t="s">
         <v>77</v>
       </c>
-      <c r="AG16" s="82"/>
-      <c r="AH16" s="83"/>
+      <c r="AG16" s="96"/>
+      <c r="AH16" s="97"/>
       <c r="AI16" s="46"/>
-      <c r="AJ16" s="81" t="s">
+      <c r="AJ16" s="95" t="s">
         <v>82</v>
       </c>
-      <c r="AK16" s="82"/>
-      <c r="AL16" s="83"/>
-    </row>
-    <row r="17" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AK16" s="96"/>
+      <c r="AL16" s="97"/>
+    </row>
+    <row r="17" spans="1:38" ht="15" thickBot="1">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2028,7 +2033,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -2045,7 +2050,7 @@
         <f>COUNTIF($E$3:$E$63, 6)</f>
         <v>1</v>
       </c>
-      <c r="I18" s="79">
+      <c r="I18" s="88">
         <f>SUM(H18:H19)*100/$H$28</f>
         <v>5.4545454545454541</v>
       </c>
@@ -2055,7 +2060,7 @@
       <c r="M18" s="16">
         <v>0</v>
       </c>
-      <c r="N18" s="84">
+      <c r="N18" s="98">
         <f>SUM(M18:M19)*100/$H$28</f>
         <v>0</v>
       </c>
@@ -2065,7 +2070,7 @@
       <c r="Q18" s="16">
         <v>0</v>
       </c>
-      <c r="R18" s="84">
+      <c r="R18" s="98">
         <f>SUM(Q18:Q19)*100/$Q$28</f>
         <v>0</v>
       </c>
@@ -2075,7 +2080,7 @@
       <c r="U18" s="16">
         <v>0</v>
       </c>
-      <c r="V18" s="79">
+      <c r="V18" s="88">
         <f>SUM(U18:U19)*100/$U$28</f>
         <v>0</v>
       </c>
@@ -2085,7 +2090,7 @@
       <c r="Y18" s="16">
         <v>0</v>
       </c>
-      <c r="Z18" s="79">
+      <c r="Z18" s="88">
         <f>SUM(Y18:Y19)*100/$Y$28</f>
         <v>16.666666666666668</v>
       </c>
@@ -2095,7 +2100,7 @@
       <c r="AC18" s="16">
         <v>0</v>
       </c>
-      <c r="AD18" s="79">
+      <c r="AD18" s="88">
         <f>SUM(AC18:AC19)*100/$AC$28</f>
         <v>0</v>
       </c>
@@ -2105,7 +2110,7 @@
       <c r="AG18" s="16">
         <v>0</v>
       </c>
-      <c r="AH18" s="79">
+      <c r="AH18" s="88">
         <f>SUM(AG18:AG19)*100/$AG$28</f>
         <v>0</v>
       </c>
@@ -2115,12 +2120,12 @@
       <c r="AK18" s="16">
         <v>1</v>
       </c>
-      <c r="AL18" s="79">
+      <c r="AL18" s="88">
         <f>SUM(AK18:AK19)*100/$AK$28</f>
         <v>16.666666666666668</v>
       </c>
     </row>
-    <row r="19" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:38" ht="15" thickBot="1">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -2137,58 +2142,58 @@
         <f>COUNTIF($E$3:$E$63, 5)</f>
         <v>2</v>
       </c>
-      <c r="I19" s="80"/>
+      <c r="I19" s="89"/>
       <c r="L19" s="18" t="s">
         <v>59</v>
       </c>
       <c r="M19" s="17">
         <v>0</v>
       </c>
-      <c r="N19" s="85"/>
+      <c r="N19" s="99"/>
       <c r="P19" s="18" t="s">
         <v>59</v>
       </c>
       <c r="Q19" s="17">
         <v>0</v>
       </c>
-      <c r="R19" s="85"/>
+      <c r="R19" s="99"/>
       <c r="T19" s="18" t="s">
         <v>59</v>
       </c>
       <c r="U19" s="17">
         <v>0</v>
       </c>
-      <c r="V19" s="80"/>
+      <c r="V19" s="89"/>
       <c r="X19" s="18" t="s">
         <v>59</v>
       </c>
       <c r="Y19" s="17">
         <v>2</v>
       </c>
-      <c r="Z19" s="80"/>
+      <c r="Z19" s="89"/>
       <c r="AB19" s="18" t="s">
         <v>59</v>
       </c>
       <c r="AC19" s="17">
         <v>0</v>
       </c>
-      <c r="AD19" s="80"/>
+      <c r="AD19" s="89"/>
       <c r="AF19" s="18" t="s">
         <v>59</v>
       </c>
       <c r="AG19" s="17">
         <v>0</v>
       </c>
-      <c r="AH19" s="80"/>
+      <c r="AH19" s="89"/>
       <c r="AJ19" s="18" t="s">
         <v>59</v>
       </c>
       <c r="AK19" s="17">
         <v>0</v>
       </c>
-      <c r="AL19" s="80"/>
-    </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL19" s="89"/>
+    </row>
+    <row r="20" spans="1:38">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -2200,7 +2205,7 @@
         <f>COUNTIF($E$3:$E$63, 4)</f>
         <v>5</v>
       </c>
-      <c r="I20" s="79">
+      <c r="I20" s="88">
         <f>SUM(H20:H21)*100/$H$28</f>
         <v>25.454545454545453</v>
       </c>
@@ -2210,7 +2215,7 @@
       <c r="M20" s="16">
         <v>0</v>
       </c>
-      <c r="N20" s="84">
+      <c r="N20" s="98">
         <f>SUM(M20:M21)*100/$H$28</f>
         <v>0</v>
       </c>
@@ -2220,7 +2225,7 @@
       <c r="Q20" s="16">
         <v>1</v>
       </c>
-      <c r="R20" s="84">
+      <c r="R20" s="98">
         <f>SUM(Q20:Q21)*100/$Q$28</f>
         <v>50</v>
       </c>
@@ -2230,7 +2235,7 @@
       <c r="U20" s="16">
         <v>0</v>
       </c>
-      <c r="V20" s="79">
+      <c r="V20" s="88">
         <f>SUM(U20:U21)*100/$U$28</f>
         <v>16.666666666666668</v>
       </c>
@@ -2240,7 +2245,7 @@
       <c r="Y20" s="16">
         <v>2</v>
       </c>
-      <c r="Z20" s="79">
+      <c r="Z20" s="88">
         <f>SUM(Y20:Y21)*100/$Y$28</f>
         <v>16.666666666666668</v>
       </c>
@@ -2250,7 +2255,7 @@
       <c r="AC20" s="16">
         <v>2</v>
       </c>
-      <c r="AD20" s="79">
+      <c r="AD20" s="88">
         <f>SUM(AC20:AC21)*100/$AC$28</f>
         <v>33.333333333333336</v>
       </c>
@@ -2260,7 +2265,7 @@
       <c r="AG20" s="16">
         <v>0</v>
       </c>
-      <c r="AH20" s="79">
+      <c r="AH20" s="88">
         <f>SUM(AG20:AG21)*100/$AG$28</f>
         <v>16.666666666666668</v>
       </c>
@@ -2270,12 +2275,12 @@
       <c r="AK20" s="16">
         <v>0</v>
       </c>
-      <c r="AL20" s="79">
+      <c r="AL20" s="88">
         <f>SUM(AK20:AK21)*100/$AK$28</f>
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="21" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:38" ht="15" thickBot="1">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -2292,58 +2297,58 @@
         <f>COUNTIF($E$3:$E$63, 3)</f>
         <v>9</v>
       </c>
-      <c r="I21" s="80"/>
+      <c r="I21" s="89"/>
       <c r="L21" s="18" t="s">
         <v>61</v>
       </c>
       <c r="M21" s="17">
         <v>0</v>
       </c>
-      <c r="N21" s="85"/>
+      <c r="N21" s="99"/>
       <c r="P21" s="18" t="s">
         <v>61</v>
       </c>
       <c r="Q21" s="17">
         <v>2</v>
       </c>
-      <c r="R21" s="85"/>
+      <c r="R21" s="99"/>
       <c r="T21" s="18" t="s">
         <v>61</v>
       </c>
       <c r="U21" s="17">
         <v>2</v>
       </c>
-      <c r="V21" s="80"/>
+      <c r="V21" s="89"/>
       <c r="X21" s="18" t="s">
         <v>61</v>
       </c>
       <c r="Y21" s="17">
         <v>0</v>
       </c>
-      <c r="Z21" s="80"/>
+      <c r="Z21" s="89"/>
       <c r="AB21" s="18" t="s">
         <v>61</v>
       </c>
       <c r="AC21" s="17">
         <v>2</v>
       </c>
-      <c r="AD21" s="80"/>
+      <c r="AD21" s="89"/>
       <c r="AF21" s="18" t="s">
         <v>61</v>
       </c>
       <c r="AG21" s="17">
         <v>1</v>
       </c>
-      <c r="AH21" s="80"/>
+      <c r="AH21" s="89"/>
       <c r="AJ21" s="18" t="s">
         <v>61</v>
       </c>
       <c r="AK21" s="17">
         <v>2</v>
       </c>
-      <c r="AL21" s="80"/>
-    </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL21" s="89"/>
+    </row>
+    <row r="22" spans="1:38">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -2360,7 +2365,7 @@
         <f>COUNTIF($E$3:$E$63, 2)</f>
         <v>10</v>
       </c>
-      <c r="I22" s="79">
+      <c r="I22" s="88">
         <f>SUM(H22:H23)*100/$H$28</f>
         <v>38.18181818181818</v>
       </c>
@@ -2370,7 +2375,7 @@
       <c r="M22" s="16">
         <v>1</v>
       </c>
-      <c r="N22" s="84">
+      <c r="N22" s="98">
         <f>SUM(M22:M23)*100/$M$28</f>
         <v>100</v>
       </c>
@@ -2380,7 +2385,7 @@
       <c r="Q22" s="16">
         <v>0</v>
       </c>
-      <c r="R22" s="84">
+      <c r="R22" s="98">
         <f>SUM(Q22:Q23)*100/$Q$28</f>
         <v>0</v>
       </c>
@@ -2390,7 +2395,7 @@
       <c r="U22" s="16">
         <v>4</v>
       </c>
-      <c r="V22" s="79">
+      <c r="V22" s="88">
         <f>SUM(U22:U23)*100/$U$28</f>
         <v>66.666666666666671</v>
       </c>
@@ -2400,7 +2405,7 @@
       <c r="Y22" s="16">
         <v>2</v>
       </c>
-      <c r="Z22" s="79">
+      <c r="Z22" s="88">
         <f>SUM(Y22:Y23)*100/$Y$28</f>
         <v>33.333333333333336</v>
       </c>
@@ -2410,7 +2415,7 @@
       <c r="AC22" s="16">
         <v>2</v>
       </c>
-      <c r="AD22" s="79">
+      <c r="AD22" s="88">
         <f>SUM(AC22:AC23)*100/$AC$28</f>
         <v>33.333333333333336</v>
       </c>
@@ -2420,7 +2425,7 @@
       <c r="AG22" s="16">
         <v>2</v>
       </c>
-      <c r="AH22" s="79">
+      <c r="AH22" s="88">
         <f>SUM(AG22:AG23)*100/$AG$28</f>
         <v>66.666666666666671</v>
       </c>
@@ -2430,12 +2435,12 @@
       <c r="AK22" s="16">
         <v>0</v>
       </c>
-      <c r="AL22" s="79">
+      <c r="AL22" s="88">
         <f>SUM(AK22:AK23)*100/$AK$28</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:38" ht="15" thickBot="1">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -2452,58 +2457,58 @@
         <f>COUNTIF($E$3:$E$63, 1)</f>
         <v>11</v>
       </c>
-      <c r="I23" s="80"/>
+      <c r="I23" s="89"/>
       <c r="L23" s="18" t="s">
         <v>57</v>
       </c>
       <c r="M23" s="17">
         <v>1</v>
       </c>
-      <c r="N23" s="85"/>
+      <c r="N23" s="99"/>
       <c r="P23" s="18" t="s">
         <v>57</v>
       </c>
       <c r="Q23" s="17">
         <v>0</v>
       </c>
-      <c r="R23" s="85"/>
+      <c r="R23" s="99"/>
       <c r="T23" s="18" t="s">
         <v>57</v>
       </c>
       <c r="U23" s="17">
         <v>4</v>
       </c>
-      <c r="V23" s="80"/>
+      <c r="V23" s="89"/>
       <c r="X23" s="18" t="s">
         <v>57</v>
       </c>
       <c r="Y23" s="17">
         <v>2</v>
       </c>
-      <c r="Z23" s="80"/>
+      <c r="Z23" s="89"/>
       <c r="AB23" s="18" t="s">
         <v>57</v>
       </c>
       <c r="AC23" s="17">
         <v>2</v>
       </c>
-      <c r="AD23" s="80"/>
+      <c r="AD23" s="89"/>
       <c r="AF23" s="18" t="s">
         <v>57</v>
       </c>
       <c r="AG23" s="17">
         <v>2</v>
       </c>
-      <c r="AH23" s="80"/>
+      <c r="AH23" s="89"/>
       <c r="AJ23" s="18" t="s">
         <v>57</v>
       </c>
       <c r="AK23" s="17">
         <v>0</v>
       </c>
-      <c r="AL23" s="80"/>
-    </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL23" s="89"/>
+    </row>
+    <row r="24" spans="1:38">
       <c r="G24" s="10" t="s">
         <v>63</v>
       </c>
@@ -2511,7 +2516,7 @@
         <f>COUNTIF($E$3:$E$63, 0)</f>
         <v>9</v>
       </c>
-      <c r="I24" s="79">
+      <c r="I24" s="88">
         <f>SUM(H24:H25)*100/$H$28</f>
         <v>25.454545454545453</v>
       </c>
@@ -2521,7 +2526,7 @@
       <c r="M24" s="16">
         <v>0</v>
       </c>
-      <c r="N24" s="84">
+      <c r="N24" s="98">
         <f>SUM(M24:M25)*100/$H$28</f>
         <v>0</v>
       </c>
@@ -2531,7 +2536,7 @@
       <c r="Q24" s="16">
         <v>2</v>
       </c>
-      <c r="R24" s="84">
+      <c r="R24" s="98">
         <f>SUM(Q24:Q25)*100/$Q$28</f>
         <v>50</v>
       </c>
@@ -2541,7 +2546,7 @@
       <c r="U24" s="16">
         <v>2</v>
       </c>
-      <c r="V24" s="79">
+      <c r="V24" s="88">
         <f>SUM(U24:U25)*100/$U$28</f>
         <v>16.666666666666668</v>
       </c>
@@ -2551,7 +2556,7 @@
       <c r="Y24" s="16">
         <v>0</v>
       </c>
-      <c r="Z24" s="79">
+      <c r="Z24" s="88">
         <f>SUM(Y24:Y25)*100/$Y$28</f>
         <v>16.666666666666668</v>
       </c>
@@ -2561,7 +2566,7 @@
       <c r="AC24" s="16">
         <v>2</v>
       </c>
-      <c r="AD24" s="79">
+      <c r="AD24" s="88">
         <f>SUM(AC24:AC25)*100/$AC$28</f>
         <v>33.333333333333336</v>
       </c>
@@ -2571,7 +2576,7 @@
       <c r="AG24" s="16">
         <v>1</v>
       </c>
-      <c r="AH24" s="79">
+      <c r="AH24" s="88">
         <f>SUM(AG24:AG25)*100/$AG$28</f>
         <v>16.666666666666668</v>
       </c>
@@ -2581,12 +2586,12 @@
       <c r="AK24" s="16">
         <v>2</v>
       </c>
-      <c r="AL24" s="79">
+      <c r="AL24" s="88">
         <f>SUM(AK24:AK25)*100/$AK$28</f>
         <v>33.333333333333336</v>
       </c>
     </row>
-    <row r="25" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:38" ht="15" thickBot="1">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -2603,58 +2608,58 @@
         <f>COUNTIF($E$3:$E$63, -1)</f>
         <v>5</v>
       </c>
-      <c r="I25" s="80"/>
+      <c r="I25" s="89"/>
       <c r="L25" s="11" t="s">
         <v>64</v>
       </c>
       <c r="M25" s="17">
         <v>0</v>
       </c>
-      <c r="N25" s="85"/>
+      <c r="N25" s="99"/>
       <c r="P25" s="11" t="s">
         <v>64</v>
       </c>
       <c r="Q25" s="17">
         <v>1</v>
       </c>
-      <c r="R25" s="85"/>
+      <c r="R25" s="99"/>
       <c r="T25" s="11" t="s">
         <v>64</v>
       </c>
       <c r="U25" s="17">
         <v>0</v>
       </c>
-      <c r="V25" s="80"/>
+      <c r="V25" s="89"/>
       <c r="X25" s="11" t="s">
         <v>64</v>
       </c>
       <c r="Y25" s="17">
         <v>2</v>
       </c>
-      <c r="Z25" s="80"/>
+      <c r="Z25" s="89"/>
       <c r="AB25" s="11" t="s">
         <v>64</v>
       </c>
       <c r="AC25" s="17">
         <v>2</v>
       </c>
-      <c r="AD25" s="80"/>
+      <c r="AD25" s="89"/>
       <c r="AF25" s="11" t="s">
         <v>64</v>
       </c>
       <c r="AG25" s="17">
         <v>0</v>
       </c>
-      <c r="AH25" s="80"/>
+      <c r="AH25" s="89"/>
       <c r="AJ25" s="11" t="s">
         <v>64</v>
       </c>
       <c r="AK25" s="17">
         <v>0</v>
       </c>
-      <c r="AL25" s="80"/>
-    </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL25" s="89"/>
+    </row>
+    <row r="26" spans="1:38">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -2671,7 +2676,7 @@
         <f>COUNTIF($E$3:$E$63, -2)</f>
         <v>2</v>
       </c>
-      <c r="I26" s="79">
+      <c r="I26" s="88">
         <f>SUM(H26:H27)*100/$H$28</f>
         <v>5.4545454545454541</v>
       </c>
@@ -2681,7 +2686,7 @@
       <c r="M26" s="47">
         <v>0</v>
       </c>
-      <c r="N26" s="84">
+      <c r="N26" s="98">
         <f>SUM(M26:M27)*100/$H$28</f>
         <v>0</v>
       </c>
@@ -2691,7 +2696,7 @@
       <c r="Q26" s="47">
         <v>0</v>
       </c>
-      <c r="R26" s="84">
+      <c r="R26" s="98">
         <f>SUM(Q26:Q27)*100/$Q$28</f>
         <v>0</v>
       </c>
@@ -2701,7 +2706,7 @@
       <c r="U26" s="47">
         <v>0</v>
       </c>
-      <c r="V26" s="79">
+      <c r="V26" s="88">
         <f>SUM(U26:U27)*100/$U$28</f>
         <v>0</v>
       </c>
@@ -2711,7 +2716,7 @@
       <c r="Y26" s="47">
         <v>2</v>
       </c>
-      <c r="Z26" s="79">
+      <c r="Z26" s="88">
         <f>SUM(Y26:Y27)*100/$Y$28</f>
         <v>16.666666666666668</v>
       </c>
@@ -2721,7 +2726,7 @@
       <c r="AC26" s="47">
         <v>0</v>
       </c>
-      <c r="AD26" s="79">
+      <c r="AD26" s="88">
         <f>SUM(AC26:AC27)*100/$AC$28</f>
         <v>0</v>
       </c>
@@ -2731,7 +2736,7 @@
       <c r="AG26" s="47">
         <v>0</v>
       </c>
-      <c r="AH26" s="79">
+      <c r="AH26" s="88">
         <f>SUM(AG26:AG27)*100/$AG$28</f>
         <v>0</v>
       </c>
@@ -2741,12 +2746,12 @@
       <c r="AK26" s="47">
         <v>0</v>
       </c>
-      <c r="AL26" s="79">
+      <c r="AL26" s="88">
         <f>SUM(AK26:AK27)*100/$AK$28</f>
         <v>16.666666666666668</v>
       </c>
     </row>
-    <row r="27" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:38" ht="15" thickBot="1">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -2763,58 +2768,58 @@
         <f>COUNTIF($E$3:$E$63, -3)</f>
         <v>1</v>
       </c>
-      <c r="I27" s="80"/>
+      <c r="I27" s="89"/>
       <c r="L27" s="11" t="s">
         <v>66</v>
       </c>
       <c r="M27" s="48">
         <v>0</v>
       </c>
-      <c r="N27" s="85"/>
+      <c r="N27" s="99"/>
       <c r="P27" s="11" t="s">
         <v>66</v>
       </c>
       <c r="Q27" s="48">
         <v>0</v>
       </c>
-      <c r="R27" s="85"/>
+      <c r="R27" s="99"/>
       <c r="T27" s="11" t="s">
         <v>66</v>
       </c>
       <c r="U27" s="48">
         <v>0</v>
       </c>
-      <c r="V27" s="80"/>
+      <c r="V27" s="89"/>
       <c r="X27" s="11" t="s">
         <v>66</v>
       </c>
       <c r="Y27" s="48">
         <v>0</v>
       </c>
-      <c r="Z27" s="80"/>
+      <c r="Z27" s="89"/>
       <c r="AB27" s="11" t="s">
         <v>66</v>
       </c>
       <c r="AC27" s="48">
         <v>0</v>
       </c>
-      <c r="AD27" s="80"/>
+      <c r="AD27" s="89"/>
       <c r="AF27" s="11" t="s">
         <v>66</v>
       </c>
       <c r="AG27" s="48">
         <v>0</v>
       </c>
-      <c r="AH27" s="80"/>
+      <c r="AH27" s="89"/>
       <c r="AJ27" s="11" t="s">
         <v>66</v>
       </c>
       <c r="AK27" s="48">
         <v>1</v>
       </c>
-      <c r="AL27" s="80"/>
-    </row>
-    <row r="28" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AL27" s="89"/>
+    </row>
+    <row r="28" spans="1:38" ht="15" thickBot="1">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2891,7 +2896,7 @@
       </c>
       <c r="AL28" s="9"/>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -2902,7 +2907,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -2913,7 +2918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -2929,7 +2934,7 @@
       </c>
       <c r="I31" s="72"/>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -2942,14 +2947,14 @@
       <c r="G32" s="74" t="s">
         <v>89</v>
       </c>
-      <c r="H32" s="91" t="s">
+      <c r="H32" s="79" t="s">
         <v>91</v>
       </c>
       <c r="I32" s="75" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -2962,12 +2967,12 @@
       <c r="G33" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="H33" s="91"/>
+      <c r="H33" s="79"/>
       <c r="I33" s="77" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -2983,7 +2988,7 @@
       </c>
       <c r="I34" s="72"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -2994,7 +2999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -3005,7 +3010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -3016,7 +3021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -3027,7 +3032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -3038,7 +3043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -3049,7 +3054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
         <v>37</v>
       </c>
@@ -3060,7 +3065,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
         <v>38</v>
       </c>
@@ -3071,7 +3076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>39</v>
       </c>
@@ -3082,7 +3087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
         <v>40</v>
       </c>
@@ -3093,7 +3098,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
         <v>41</v>
       </c>
@@ -3104,7 +3109,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9">
       <c r="A47" t="s">
         <v>42</v>
       </c>
@@ -3115,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>43</v>
       </c>
@@ -3126,7 +3131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>44</v>
       </c>
@@ -3137,7 +3142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>45</v>
       </c>
@@ -3148,7 +3153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>46</v>
       </c>
@@ -3159,7 +3164,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -3170,7 +3175,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -3181,7 +3186,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>49</v>
       </c>
@@ -3192,7 +3197,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>50</v>
       </c>
@@ -3203,7 +3208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>51</v>
       </c>
@@ -3214,7 +3219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>52</v>
       </c>
@@ -3225,7 +3230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>53</v>
       </c>
@@ -3236,7 +3241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>54</v>
       </c>
@@ -3247,7 +3252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>55</v>
       </c>
@@ -3258,48 +3263,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:4">
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="H5:I6"/>
-    <mergeCell ref="H7:I8"/>
-    <mergeCell ref="H9:I10"/>
-    <mergeCell ref="H11:I12"/>
-    <mergeCell ref="H13:I14"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="AB16:AD16"/>
-    <mergeCell ref="AJ16:AL16"/>
-    <mergeCell ref="AF16:AH16"/>
-    <mergeCell ref="AF3:AH3"/>
-    <mergeCell ref="AJ3:AL3"/>
-    <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="R24:R25"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="L16:N16"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="T16:V16"/>
-    <mergeCell ref="V22:V23"/>
-    <mergeCell ref="V24:V25"/>
-    <mergeCell ref="V26:V27"/>
+    <mergeCell ref="AD18:AD19"/>
+    <mergeCell ref="AD20:AD21"/>
+    <mergeCell ref="AD22:AD23"/>
+    <mergeCell ref="AD24:AD25"/>
+    <mergeCell ref="AD26:AD27"/>
+    <mergeCell ref="AL18:AL19"/>
+    <mergeCell ref="AL20:AL21"/>
+    <mergeCell ref="AL22:AL23"/>
+    <mergeCell ref="AL24:AL25"/>
+    <mergeCell ref="AL26:AL27"/>
+    <mergeCell ref="AH18:AH19"/>
+    <mergeCell ref="AH20:AH21"/>
+    <mergeCell ref="AH22:AH23"/>
+    <mergeCell ref="AH24:AH25"/>
+    <mergeCell ref="AH26:AH27"/>
     <mergeCell ref="X16:Z16"/>
     <mergeCell ref="N22:N23"/>
     <mergeCell ref="N24:N25"/>
@@ -3316,24 +3306,43 @@
     <mergeCell ref="V20:V21"/>
     <mergeCell ref="N18:N19"/>
     <mergeCell ref="N20:N21"/>
-    <mergeCell ref="AH18:AH19"/>
-    <mergeCell ref="AH20:AH21"/>
-    <mergeCell ref="AH22:AH23"/>
-    <mergeCell ref="AH24:AH25"/>
-    <mergeCell ref="AH26:AH27"/>
-    <mergeCell ref="AL18:AL19"/>
-    <mergeCell ref="AL20:AL21"/>
-    <mergeCell ref="AL22:AL23"/>
-    <mergeCell ref="AL24:AL25"/>
-    <mergeCell ref="AL26:AL27"/>
-    <mergeCell ref="AD18:AD19"/>
-    <mergeCell ref="AD20:AD21"/>
-    <mergeCell ref="AD22:AD23"/>
-    <mergeCell ref="AD24:AD25"/>
-    <mergeCell ref="AD26:AD27"/>
+    <mergeCell ref="R24:R25"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="T16:V16"/>
+    <mergeCell ref="V22:V23"/>
+    <mergeCell ref="V24:V25"/>
+    <mergeCell ref="V26:V27"/>
+    <mergeCell ref="AB16:AD16"/>
+    <mergeCell ref="AJ16:AL16"/>
+    <mergeCell ref="AF16:AH16"/>
+    <mergeCell ref="AF3:AH3"/>
+    <mergeCell ref="AJ3:AL3"/>
+    <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="X3:Z3"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="H5:I6"/>
+    <mergeCell ref="H7:I8"/>
+    <mergeCell ref="H9:I10"/>
+    <mergeCell ref="H11:I12"/>
+    <mergeCell ref="H13:I14"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="I26:I27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3343,9 +3352,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3355,8 +3369,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>